<commit_message>
Adding spring jdbc & spring mvc
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Raj\git\edureka_spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A12337-DE05-484B-9288-151412AC4DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4403341-12AF-44D1-87DE-5DF6D2FA21CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37935" yWindow="3720" windowWidth="13830" windowHeight="7965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Topics</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Transactions using Transaction Manager Bean</t>
+  </si>
+  <si>
+    <t>IOC tells let the client class do not take object creation responsibility, let some external component create the objects required for the client and give it. This will give loose coupling.</t>
   </si>
 </sst>
 </file>
@@ -268,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -280,7 +283,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -662,8 +664,8 @@
   </sheetPr>
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -994,7 +996,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="7" t="s">
+      <c r="B64" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="3">
@@ -1002,7 +1004,7 @@
       </c>
     </row>
     <row r="65" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C65" s="3">
@@ -1010,7 +1012,7 @@
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="7" t="s">
+      <c r="B66" t="s">
         <v>62</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -1025,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71CDDC4-B53F-464F-9F5A-51154B9FF1E5}">
-  <dimension ref="A2:A12"/>
+  <dimension ref="A2:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,28 +1048,33 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>